<commit_message>
success filename 20.3319 task 0814
</commit_message>
<xml_diff>
--- a/Arif 0814/Arif 0814.xlsx
+++ b/Arif 0814/Arif 0814.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif 0814\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7432CB29-E494-42E7-8CAD-489633025CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B0E451-1749-45C5-8514-6C6B76349D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -239,7 +239,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,6 +380,21 @@
       <color theme="1"/>
       <name val="Eurostile"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Eurostile"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -439,7 +454,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -563,10 +578,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -848,7 +869,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -983,41 +1004,41 @@
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
     </row>
-    <row r="7" spans="1:8" s="44" customFormat="1" ht="27" customHeight="1">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:8" s="46" customFormat="1" ht="27" customHeight="1">
+      <c r="A7" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-    </row>
-    <row r="8" spans="1:8" ht="27" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="F7" s="43"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+    </row>
+    <row r="8" spans="1:8" s="46" customFormat="1" ht="27" customHeight="1">
+      <c r="A8" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="34"/>
+      <c r="C8" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
     </row>
     <row r="9" spans="1:8" s="30" customFormat="1" ht="27" customHeight="1">
       <c r="A9" s="15" t="s">

</xml_diff>

<commit_message>
success filename 20.3320 task 0814
</commit_message>
<xml_diff>
--- a/Arif 0814/Arif 0814.xlsx
+++ b/Arif 0814/Arif 0814.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif 0814\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B0E451-1749-45C5-8514-6C6B76349D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8507BCC1-6C84-401A-8E3F-D67C05DB2BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
   <si>
     <t>FileName</t>
   </si>
@@ -234,6 +234,9 @@
   <si>
     <t>26</t>
   </si>
+  <si>
+    <t>64</t>
+  </si>
 </sst>
 </file>
 
@@ -245,6 +248,20 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -380,21 +397,6 @@
       <color theme="1"/>
       <name val="Eurostile"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Eurostile"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -450,62 +452,95 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -514,35 +549,14 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
@@ -550,44 +564,26 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -869,7 +865,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1004,41 +1000,45 @@
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
     </row>
-    <row r="7" spans="1:8" s="46" customFormat="1" ht="27" customHeight="1">
-      <c r="A7" s="34" t="s">
+    <row r="7" spans="1:8" s="43" customFormat="1" ht="27" customHeight="1">
+      <c r="A7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="43" t="s">
+      <c r="B7" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-    </row>
-    <row r="8" spans="1:8" s="46" customFormat="1" ht="27" customHeight="1">
-      <c r="A8" s="34" t="s">
+      <c r="F7" s="16"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:8" s="44" customFormat="1" ht="27" customHeight="1">
+      <c r="A8" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="43" t="s">
+      <c r="B8" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" s="30" customFormat="1" ht="27" customHeight="1">
       <c r="A9" s="15" t="s">

</xml_diff>